<commit_message>
skompletowane czesci, wybrane rezystory, kondensator przy wejsciu
</commit_message>
<xml_diff>
--- a/części.xlsx
+++ b/części.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f422b1b9f3a216ed/Programowanie/Roboty/Linefollower-2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Programowanie\Roboty\Linefollower-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>Botland</t>
   </si>
@@ -54,9 +54,6 @@
     <t>LED RGB</t>
   </si>
   <si>
-    <t>Kwarc 16MHz</t>
-  </si>
-  <si>
     <t>LED Biała</t>
   </si>
   <si>
@@ -102,20 +99,59 @@
     <t>Nie wybrane</t>
   </si>
   <si>
-    <t>gniazdo miniusb</t>
-  </si>
-  <si>
     <t>przelacznik on/off</t>
   </si>
   <si>
-    <t>rezystory np. dla rgb</t>
+    <t>USB typ B smd mini</t>
+  </si>
+  <si>
+    <t>R150k</t>
+  </si>
+  <si>
+    <t>R13k</t>
+  </si>
+  <si>
+    <t>R22k</t>
+  </si>
+  <si>
+    <t>R62k</t>
+  </si>
+  <si>
+    <t>KTIR0711S</t>
+  </si>
+  <si>
+    <t>C22pF</t>
+  </si>
+  <si>
+    <t>C100nF</t>
+  </si>
+  <si>
+    <t>C10nF</t>
+  </si>
+  <si>
+    <t>C4,7</t>
+  </si>
+  <si>
+    <t>C10uF</t>
+  </si>
+  <si>
+    <t>LM1117 3.3V</t>
+  </si>
+  <si>
+    <t>LM1117 5V</t>
+  </si>
+  <si>
+    <t>Kwarc 8MHz</t>
+  </si>
+  <si>
+    <t>mocowanie silnika</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,8 +160,17 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -144,6 +189,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -157,10 +208,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -477,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -510,7 +563,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -539,24 +592,48 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>1.95</v>
+      </c>
       <c r="D5">
         <f>B5*C5</f>
-        <v>0</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>39</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>17.899999999999999</v>
       </c>
       <c r="D6">
-        <f>SUM(D3:D5)</f>
-        <v>159.80000000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>24</v>
-      </c>
+        <f>B6*C6</f>
+        <v>17.899999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4">
+        <f>SUM(D3:D6)</f>
+        <v>197.20000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C11" s="3"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -565,30 +642,26 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -632,13 +705,13 @@
         <v>13.99</v>
       </c>
       <c r="D3">
-        <f>B3*C3</f>
+        <f t="shared" ref="D3:D29" si="0">B3*C3</f>
         <v>27.98</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -647,7 +720,7 @@
         <v>0.49</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D18" si="0">B4*C4</f>
+        <f t="shared" si="0"/>
         <v>1.47</v>
       </c>
     </row>
@@ -656,34 +729,34 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>0.99</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>2.9699999999999998</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6">
-        <v>2.2000000000000002</v>
+        <v>1.8</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>6.6000000000000005</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -698,7 +771,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -713,22 +786,22 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9">
         <v>2.5</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>7.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -743,22 +816,22 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C11">
         <v>0.69</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>3.4499999999999997</v>
+        <v>2.0699999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -773,22 +846,22 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>0.3</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -803,7 +876,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -818,7 +891,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16">
         <v>5</v>
@@ -832,18 +905,209 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>0.3</v>
+      </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>26</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>0.3</v>
       </c>
       <c r="D18">
-        <f>B18*C18+SUM(D3:D17)</f>
-        <v>65.66</v>
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>0.3</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>0.3</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>0.3</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>1.01</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>3.0300000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>0.39</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>0.39</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>0.45</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>0.85</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>0.8</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>1.8</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>1.35</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4">
+        <f>B30*C30+SUM(D3:D29)</f>
+        <v>74.649999999999963</v>
       </c>
     </row>
   </sheetData>

</xml_diff>